<commit_message>
sửa giao diện import export người dùng tổ chức
</commit_message>
<xml_diff>
--- a/src/assets/upload/import_to_chuc.xlsx
+++ b/src/assets/upload/import_to_chuc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP Probook 440G8\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\econtract-web\src\assets\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A16AC0B-4BCE-4764-A1DD-4AC3E251313E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53232CA-746F-4536-AE04-28FDCC19B696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{70240AC9-0F1E-4929-B952-C18F84654838}"/>
   </bookViews>
@@ -47,10 +47,10 @@
     <t>Mã số thuế</t>
   </si>
   <si>
-    <t xml:space="preserve">Mã tổ chức cấp trên(*)  </t>
-  </si>
-  <si>
     <t>Fax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID tổ chức cấp trên(*)  </t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,10 +437,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
sửa file import tổ chức
</commit_message>
<xml_diff>
--- a/src/assets/upload/import_to_chuc.xlsx
+++ b/src/assets/upload/import_to_chuc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\econtract-web\src\assets\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thang\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BE9C54-F5C1-4FE4-ACF8-9275A6C11981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29406FE-D9D3-4F93-B226-4727B70B9374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{70240AC9-0F1E-4929-B952-C18F84654838}"/>
   </bookViews>
@@ -401,26 +401,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BBC2C0-B888-4BD4-9E49-370C16BBA5F4}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -432,15 +433,9 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>